<commit_message>
run program and send certificate
</commit_message>
<xml_diff>
--- a/certificate_pdf/data/Students Inquiry file 2022-2023.xlsx
+++ b/certificate_pdf/data/Students Inquiry file 2022-2023.xlsx
@@ -7191,11 +7191,11 @@
   <dimension ref="A1:Y1776"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B218" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1268" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A218" activeCellId="0" sqref="A218"/>
-      <selection pane="bottomRight" activeCell="A227" activeCellId="0" sqref="A227:D227"/>
+      <selection pane="bottomLeft" activeCell="A1268" activeCellId="0" sqref="A1268"/>
+      <selection pane="bottomRight" activeCell="A1277" activeCellId="0" sqref="A1277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>